<commit_message>
Add options for sheet name and index; default delim is comma; better handling of general numeric format
</commit_message>
<xml_diff>
--- a/test_data/empty_cols.xlsx
+++ b/test_data/empty_cols.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">c</t>
   </si>
   <si>
     <t xml:space="preserve">a</t>
@@ -49,6 +46,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -133,7 +131,7 @@
   <dimension ref="B2:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -147,19 +145,19 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
-        <v>1</v>
+      <c r="B3" s="0" t="n">
+        <v>2.66666156237642</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="0" t="s">
         <v>3</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Empty cells with formatting are detected as blank. Fix tab vs spaces
</commit_message>
<xml_diff>
--- a/test_data/empty_cols.xlsx
+++ b/test_data/empty_cols.xlsx
@@ -72,12 +72,19 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -106,8 +113,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -128,10 +139,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -139,24 +150,27 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D2" s="0" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
         <v>2.66666156237642</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E5" s="0" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>